<commit_message>
Mini corrections: BS no intermediate result; SO delivery interval
</commit_message>
<xml_diff>
--- a/codebook/data_intervals_elections2023.xlsx
+++ b/codebook/data_intervals_elections2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\wd-poku\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFE84B2-68F3-44FD-A489-16056D702CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A4A236-90F4-44F9-B1EE-927ABEAE7AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="1575" windowWidth="22980" windowHeight="12195" xr2:uid="{F8D761AE-B0C5-436F-B6B6-584C4068E82E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{F8D761AE-B0C5-436F-B6B6-584C4068E82E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
   <si>
     <t>Nr.</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Intervalle de transfert: toutes les 30 minutes</t>
   </si>
   <si>
-    <t>Intervalle de transfert: toutes les 5 minutes</t>
-  </si>
-  <si>
     <t>Transfert multiple: 1-2 transferts intermédiaires, puis résultat final</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
   </si>
   <si>
     <t>Lieferintervall: ca. alle 30 Minuten (manuell ausgelöst)</t>
-  </si>
-  <si>
-    <t>Lieferintervall: alle 5 Minuten</t>
   </si>
   <si>
     <t>Lieferintervall: alle 5 Minuten, sofern neue Gemeindeergebnisse vorhanden sind</t>
@@ -841,7 +835,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -864,7 +858,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
@@ -889,7 +883,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>34</v>
@@ -903,7 +897,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>36</v>
@@ -945,10 +939,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="9" customFormat="1" ht="15" thickBot="1">
@@ -987,10 +981,10 @@
         <v>24</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="9" customFormat="1" ht="15" thickBot="1">
@@ -1001,24 +995,24 @@
         <v>11</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="9" customFormat="1" ht="15" thickBot="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="9" customFormat="1" ht="29.25" thickBot="1">
       <c r="A12" s="6">
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>40</v>
+      <c r="C12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="9" customFormat="1" ht="15" thickBot="1">
@@ -1043,7 +1037,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>38</v>
@@ -1057,10 +1051,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="9" customFormat="1" ht="15" thickBot="1">
@@ -1099,10 +1093,10 @@
         <v>30</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="9" customFormat="1" ht="15" thickBot="1">
@@ -1113,10 +1107,10 @@
         <v>26</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="9" customFormat="1" ht="43.5" thickBot="1">
@@ -1130,7 +1124,7 @@
         <v>32</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="9" customFormat="1" ht="15" thickBot="1">
@@ -1141,7 +1135,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>39</v>
@@ -1155,10 +1149,10 @@
         <v>27</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="9" customFormat="1" ht="29.25" thickBot="1">
@@ -1169,10 +1163,10 @@
         <v>13</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="9" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
@@ -1183,10 +1177,10 @@
         <v>15</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="9" customFormat="1" ht="15" thickBot="1">
@@ -1197,10 +1191,10 @@
         <v>21</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="9" customFormat="1" ht="15" thickBot="1">
@@ -1225,7 +1219,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>38</v>

</xml_diff>